<commit_message>
updated copy, work under progress
</commit_message>
<xml_diff>
--- a/src/test/resources/loginTestData.xlsx
+++ b/src/test/resources/loginTestData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\ideaWorkspace\SeleniumJava\SeleniumJava\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB3A1D0-94A1-41FB-8D3E-089B0FF9630F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F35134-D444-446E-9D74-703C88947D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A4EF1EA4-E433-4A5C-8855-116FEB7F7C43}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>S.NO</t>
   </si>
@@ -61,12 +61,33 @@
   </si>
   <si>
     <t>pass3</t>
+  </si>
+  <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>asdasdasdasd</t>
+  </si>
+  <si>
+    <t>Your username is invalid!
+×</t>
+  </si>
+  <si>
+    <t>You logged into a secure area!
+×</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -437,14 +458,14 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.85546875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.140625"/>
+    <col min="4" max="4" customWidth="true" width="16.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -471,7 +492,9 @@
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -483,7 +506,9 @@
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -495,7 +520,9 @@
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -507,7 +534,9 @@
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>